<commit_message>
All Readme updates and some extraneous file deletions
</commit_message>
<xml_diff>
--- a/Range Utilities/Range Utilities.xlsx
+++ b/Range Utilities/Range Utilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\ObsidianVaults\Lambda-Update-Project\Lambda-Development\Range Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Lambda-Development\Range Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE45A7DA-30D3-48F8-A6F2-EDC42A0775C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336AC614-E9EC-40D5-8F34-26DC7B483DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="2010" windowWidth="28185" windowHeight="14190" activeTab="1" xr2:uid="{D80B3487-635B-2E4E-BDFF-D2F369F38B28}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="26370" windowHeight="11295" activeTab="1" xr2:uid="{D80B3487-635B-2E4E-BDFF-D2F369F38B28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sums" sheetId="5" r:id="rId1"/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="56">
   <si>
     <t>Inputs</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Martin</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="5">
+  <wetp:taskpane dockstate="right" visibility="0" width="390" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1122,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71C20DC-E365-AB44-9566-48942D550AEB}">
-  <dimension ref="B2:J53"/>
+  <dimension ref="B2:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.75"/>
@@ -1167,15 +1170,15 @@
         <v>YecSmjE</v>
       </c>
       <c r="H3" s="2" t="str" cm="1">
-        <f t="array" ref="H3:H4">_xlfn._xlws.SORT(RANGE_INTERSECT(B3,C3,,1))</f>
+        <f t="array" ref="H3:H37">_xlfn._xlws.SORT(RANGE_INTERSECT(B3:B53,C3:C37,,1))</f>
         <v># U ∩ A</v>
       </c>
       <c r="I3" s="2" t="str" cm="1">
-        <f t="array" ref="I3:I5">RANGE_SYMDIFF(B3,C4,1,1)</f>
+        <f t="array" ref="I3:I21">RANGE_SYMDIFF(B3:B53,C3:C37,1,1)</f>
         <v># U △ A</v>
       </c>
       <c r="J3" s="2" t="str" cm="1">
-        <f t="array" ref="J3:J5">RANGE_UNION(B3,C3:C4,1,1)</f>
+        <f t="array" ref="J3:J55">RANGE_UNION(B3:B53,C3:C37,1,1)</f>
         <v># U ∪ A</v>
       </c>
     </row>
@@ -1187,13 +1190,13 @@
         <v>3</v>
       </c>
       <c r="H4" s="2" t="str">
-        <v>MDJhawJ</v>
+        <v>cgndMFb</v>
       </c>
       <c r="I4" s="2" t="str">
-        <v>MDJhawJ</v>
+        <v>AEuwOuE</v>
       </c>
       <c r="J4" s="2" t="str">
-        <v>MDJhawJ</v>
+        <v>AEuwOuE</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -1203,11 +1206,14 @@
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="H5" s="2" t="str">
+        <v>DqeANmO</v>
+      </c>
       <c r="I5" s="2" t="str">
-        <v>YecSmjE</v>
+        <v>BtSOrAZ</v>
       </c>
       <c r="J5" s="2" t="str">
-        <v>YecSmjE</v>
+        <v>BtSOrAZ</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -1219,7 +1225,16 @@
       </c>
       <c r="G6" s="2" t="str">
         <f ca="1">_xlfn.FORMULATEXT(F21)</f>
-        <v>=RANGE_COMPLEMENT(B4,C3,"ABS",1)</v>
+        <v>=RANGE_COMPLEMENT(B3,C4,"ABS",1)</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <v>DzyrDHF</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <v>BwCMrXl</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <v>BwCMrXl</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -1229,6 +1244,15 @@
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H7" s="2" t="str">
+        <v>EbMvEol</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <v>CcsRZvY</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <v>CcsRZvY</v>
+      </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="2" t="s">
@@ -1237,6 +1261,15 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H8" s="2" t="str">
+        <v>FdoiTSk</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <v>EFmUoES</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <v>cgndMFb</v>
+      </c>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="2" t="s">
@@ -1245,6 +1278,15 @@
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H9" s="2" t="str">
+        <v>fKFyxrT</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <v>eOYSkqv</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <v>DqeANmO</v>
+      </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="2" t="s">
@@ -1253,12 +1295,14 @@
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2" t="str" cm="1">
-        <f t="array" ref="G10:H14">RANGE_ISIN(B3:B13,C6:C10,3)</f>
-        <v>JOmcBux</v>
-      </c>
-      <c r="H10" s="2" t="b">
-        <v>1</v>
+      <c r="H10" s="2" t="str">
+        <v>GbvASTj</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <v>fNgeThR</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <v>DzyrDHF</v>
       </c>
     </row>
     <row r="11" spans="2:10">
@@ -1268,11 +1312,14 @@
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="2" t="str">
-        <v>GbvASTj</v>
-      </c>
-      <c r="H11" s="2" t="b">
-        <v>1</v>
+      <c r="H11" s="2" t="str">
+        <v>gEYsvkJ</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <v>fZalsJC</v>
+      </c>
+      <c r="J11" s="2" t="str">
+        <v>EbMvEol</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -1282,11 +1329,14 @@
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="2" t="str">
-        <v>VvCPWAG</v>
-      </c>
-      <c r="H12" s="2" t="b">
-        <v>1</v>
+      <c r="H12" s="2" t="str">
+        <v>GsYrWhl</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <v>KSqFpfB</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <v>EFmUoES</v>
       </c>
     </row>
     <row r="13" spans="2:10">
@@ -1296,11 +1346,14 @@
       <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="2" t="str">
-        <v>YqFYPAD</v>
-      </c>
-      <c r="H13" s="2" t="b">
-        <v>1</v>
+      <c r="H13" s="2" t="str">
+        <v>JNOyLdL</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <v>lXabdvD</v>
+      </c>
+      <c r="J13" s="2" t="str">
+        <v>eOYSkqv</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -1310,11 +1363,14 @@
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="2" t="str">
-        <v>WbzRAmU</v>
-      </c>
-      <c r="H14" s="2" t="b">
-        <v>1</v>
+      <c r="H14" s="2" t="str">
+        <v>JOmcBux</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <v>Martin</v>
+      </c>
+      <c r="J14" s="2" t="str">
+        <v>FdoiTSk</v>
       </c>
     </row>
     <row r="15" spans="2:10">
@@ -1322,7 +1378,16 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>55</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <v>KqxxeAy</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <v>nhoGtqh</v>
+      </c>
+      <c r="J15" s="2" t="str">
+        <v>fKFyxrT</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -1332,40 +1397,85 @@
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="H16" s="2" t="str">
+        <v>KWeqfrO</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <v>nSLSQCl</v>
+      </c>
+      <c r="J16" s="2" t="str">
+        <v>fNgeThR</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="H17" s="2" t="str">
+        <v>MCABMpu</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <v>OaRKZLh</v>
+      </c>
+      <c r="J17" s="2" t="str">
+        <v>fZalsJC</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="H18" s="2" t="str">
+        <v>MDJhawJ</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <v>VzjTCZU</v>
+      </c>
+      <c r="J18" s="2" t="str">
+        <v>GbvASTj</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="2:6">
+      <c r="H19" s="2" t="str">
+        <v>MGxUeKM</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <v>XDGMJbV</v>
+      </c>
+      <c r="J19" s="2" t="str">
+        <v>gEYsvkJ</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="H20" s="2" t="str">
+        <v>MUynYmh</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <v>xTjhfcE</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <v>GsYrWhl</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1373,11 +1483,20 @@
         <v>45</v>
       </c>
       <c r="F21" s="2" t="str" cm="1">
-        <f t="array" ref="F21:F22">RANGE_COMPLEMENT(B4,C3,"ABS",1)</f>
+        <f t="array" ref="F21:F22">RANGE_COMPLEMENT(B3,C4,"ABS",1)</f>
         <v># A \\ U</v>
       </c>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="H21" s="2" t="str">
+        <v>ONKUupJ</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <v>zQTpqqa</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <v>JNOyLdL</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1385,207 +1504,408 @@
         <v>47</v>
       </c>
       <c r="F22" s="2" t="str">
-        <v>MDJhawJ</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
+        <v>YecSmjE</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <v>qfkGjdP</v>
+      </c>
+      <c r="J22" s="2" t="str">
+        <v>JOmcBux</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="2:6">
+      <c r="H23" s="2" t="str">
+        <v>rIABHdw</v>
+      </c>
+      <c r="J23" s="2" t="str">
+        <v>KqxxeAy</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="2:6">
+      <c r="H24" s="2" t="str">
+        <v>rNVETir</v>
+      </c>
+      <c r="J24" s="2" t="str">
+        <v>KSqFpfB</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:6">
+      <c r="H25" s="2" t="str">
+        <v>RQuGImR</v>
+      </c>
+      <c r="J25" s="2" t="str">
+        <v>KWeqfrO</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
       <c r="B26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="2:6">
+      <c r="H26" s="2" t="str">
+        <v>TEEuFYL</v>
+      </c>
+      <c r="J26" s="2" t="str">
+        <v>lXabdvD</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="H27" s="2" t="str">
+        <v>ukAysyB</v>
+      </c>
+      <c r="J27" s="2" t="str">
+        <v>Martin</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
       <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="H28" s="2" t="str">
+        <v>ukGHTeZ</v>
+      </c>
+      <c r="J28" s="2" t="str">
+        <v>MCABMpu</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
       <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="2:6">
+      <c r="H29" s="2" t="str">
+        <v>UNKFFCk</v>
+      </c>
+      <c r="J29" s="2" t="str">
+        <v>MDJhawJ</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
       <c r="B30" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="2:6">
+      <c r="H30" s="2" t="str">
+        <v>VvCPWAG</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <v>MGxUeKM</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
       <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="2:6">
+      <c r="H31" s="2" t="str">
+        <v>vVnLLAp</v>
+      </c>
+      <c r="J31" s="2" t="str">
+        <v>MUynYmh</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
       <c r="B32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="2:3">
+      <c r="H32" s="2" t="str">
+        <v>WbzRAmU</v>
+      </c>
+      <c r="J32" s="2" t="str">
+        <v>nhoGtqh</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
       <c r="B33" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="2:3">
+      <c r="H33" s="2" t="str">
+        <v>WXKSpKA</v>
+      </c>
+      <c r="J33" s="2" t="str">
+        <v>nSLSQCl</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
       <c r="B34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="2:3">
+      <c r="H34" s="2" t="str">
+        <v>xcgbaoU</v>
+      </c>
+      <c r="J34" s="2" t="str">
+        <v>OaRKZLh</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
       <c r="B35" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="36" spans="2:3">
+      <c r="H35" s="2" t="str">
+        <v>XxcwTqf</v>
+      </c>
+      <c r="J35" s="2" t="str">
+        <v>ONKUupJ</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
       <c r="B36" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="2:3">
+      <c r="H36" s="2" t="str">
+        <v>YecSmjE</v>
+      </c>
+      <c r="J36" s="2" t="str">
+        <v>qfkGjdP</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
       <c r="B37" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="38" spans="2:3">
+      <c r="H37" s="2" t="str">
+        <v>YqFYPAD</v>
+      </c>
+      <c r="J37" s="2" t="str">
+        <v>rIABHdw</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
       <c r="B38" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="2:3">
+      <c r="J38" s="2" t="str">
+        <v>rNVETir</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
       <c r="B39" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="2:3">
+      <c r="J39" s="2" t="str">
+        <v>RQuGImR</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
       <c r="B40" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="2:3">
+      <c r="J40" s="2" t="str">
+        <v>TEEuFYL</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
       <c r="B41" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="2:3">
+      <c r="J41" s="2" t="str">
+        <v>ukAysyB</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
       <c r="B42" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="2:3">
+      <c r="J42" s="2" t="str">
+        <v>ukGHTeZ</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
       <c r="B43" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="2:3">
+      <c r="J43" s="2" t="str">
+        <v>UNKFFCk</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
       <c r="B44" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="45" spans="2:3">
+      <c r="J44" s="2" t="str">
+        <v>VvCPWAG</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
       <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="2:3">
+      <c r="J45" s="2" t="str">
+        <v>vVnLLAp</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
       <c r="B46" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="47" spans="2:3">
+      <c r="J46" s="2" t="str">
+        <v>VzjTCZU</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
       <c r="B47" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="2:3">
+      <c r="J47" s="2" t="str">
+        <v>WbzRAmU</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
       <c r="B48" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="49" spans="2:2">
+      <c r="J48" s="2" t="str">
+        <v>WXKSpKA</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
       <c r="B49" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="2:2">
+      <c r="J49" s="2" t="str">
+        <v>xcgbaoU</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
       <c r="B50" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="2:2">
+      <c r="J50" s="2" t="str">
+        <v>XDGMJbV</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
       <c r="B51" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="2:2">
+      <c r="J51" s="2" t="str">
+        <v>xTjhfcE</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
       <c r="B52" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="2:2">
+      <c r="J52" s="2" t="str">
+        <v>XxcwTqf</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
       <c r="B53" s="2" t="s">
         <v>52</v>
+      </c>
+      <c r="J53" s="2" t="str">
+        <v>YecSmjE</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="J54" s="2" t="str">
+        <v>YqFYPAD</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="J55" s="2" t="str">
+        <v>zQTpqqa</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="G56" s="2" t="str" cm="1">
+        <f t="array" ref="G56:H60">RANGE_ISIN(B3:B13,C6:C10,3)</f>
+        <v>JOmcBux</v>
+      </c>
+      <c r="H56" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="G57" s="2" t="str">
+        <v>GbvASTj</v>
+      </c>
+      <c r="H57" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="G58" s="2" t="str">
+        <v>VvCPWAG</v>
+      </c>
+      <c r="H58" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="G59" s="2" t="str">
+        <v>YqFYPAD</v>
+      </c>
+      <c r="H59" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="G60" s="2" t="str">
+        <v>WbzRAmU</v>
+      </c>
+      <c r="H60" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="G63" s="2" t="str" cm="1">
+        <f t="array" ref="G63">RANGE_ANALYSIS(B3:B53,C3:C37)</f>
+        <v>INTER</v>
       </c>
     </row>
   </sheetData>

</xml_diff>